<commit_message>
Add loop for request
Requests function put in try/catch with a while loop, always eventually manages to pull data from Amazon despite attempts to block bots. Also, creates conditional formatting within the Excel 'Logged' sheet, fills in cells red that don't match the 'Actual' sheet data. Next steps: read urls from Excel sheet, fix scraping of drop down menu styles in Amazon.
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -44,12 +44,56 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <bgColor rgb="00ff847e"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <bgColor rgb="00FF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <bgColor rgb="00800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEE1111"/>
+        <bgColor rgb="FFEE1111"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEE1100"/>
+        <bgColor rgb="FFEE1111"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFEE11"/>
+        <bgColor rgb="00FFEE11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+        <bgColor rgb="00FFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -80,7 +124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -88,27 +132,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -485,7 +521,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -522,107 +558,107 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="12" t="inlineStr">
         <is>
           <t>Outward Hound Hide-A-Squirrel Squeaky Puzzle Plush Dog Toy - Hide and Seek Activity for Dogs</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="9" t="inlineStr">
+        <is>
+          <t>Visit the Outward Hound Store</t>
+        </is>
+      </c>
+      <c r="C2" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="D2" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="12" t="inlineStr">
+        <is>
+          <t>Outward Hound, Lightweight Dog Backpacks, Carriers &amp; Pet Travel Products</t>
+        </is>
+      </c>
+      <c r="B3" s="12" t="inlineStr">
         <is>
           <t>Outward Hound</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>7</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="C3" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Outward Hound, Lightweight Dog Backpacks, Carriers &amp; Pet Travel Products</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="D3" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" s="12" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="12" t="inlineStr">
+        <is>
+          <t>Nina Ottosson By Outward Hound - Interactive Puzzle Game Dog Toys</t>
+        </is>
+      </c>
+      <c r="B4" s="9" t="inlineStr">
+        <is>
+          <t>Visit the Outward Hound Store</t>
+        </is>
+      </c>
+      <c r="C4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="12" t="inlineStr">
+        <is>
+          <t>Outward Hound Fun Feeder Dog Bowl</t>
+        </is>
+      </c>
+      <c r="B5" s="12" t="inlineStr">
         <is>
           <t>Outward Hound</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C5" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D5" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="E3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Nina Ottosson By Outward Hound - Interactive Puzzle Game Dog Toys</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="E5" s="12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="12" t="inlineStr">
+        <is>
+          <t>Outward Hound (4 pc. Multi-Pack) Invincibles Plush Stuffing-Less Dog Toys with Squeaker</t>
+        </is>
+      </c>
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>Visit the Outward Hound Store</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>4</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Outward Hound Fun Feeder Dog Bowl</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Visit the Outward Hound Store</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>6</v>
-      </c>
-      <c r="D5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Outward Hound (4 pc. Multi-Pack) Invincibles Plush Stuffing-Less Dog Toys with Squeaker</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Outward Hound</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
+      <c r="C6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -641,7 +677,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fixed Dropdown Style Option, reads URLs from Excel
Scrapes data from dropdown menu for style options now too. Reads URLs in from the last row of 'Actual' Excel sheet. Next steps: add more products and find bugs
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Logged'!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Actual'!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Actual'!$A$1:$F$6</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -44,32 +44,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <bgColor rgb="00ff847e"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <bgColor rgb="00FF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <bgColor rgb="00800000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -79,14 +59,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEE1100"/>
-        <bgColor rgb="FFEE1111"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFEE11"/>
-        <bgColor rgb="00FFEE11"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -124,7 +98,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -134,12 +108,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,7 +491,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -531,134 +501,134 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Product Title</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>Brand</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Style</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Size</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>Color</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="inlineStr">
+      <c r="A2" s="8" t="inlineStr">
         <is>
           <t>Outward Hound Hide-A-Squirrel Squeaky Puzzle Plush Dog Toy - Hide and Seek Activity for Dogs</t>
         </is>
       </c>
-      <c r="B2" s="9" t="inlineStr">
+      <c r="B2" s="8" t="inlineStr">
+        <is>
+          <t>Outward Hound</t>
+        </is>
+      </c>
+      <c r="C2" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="D2" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>Outward Hound, Lightweight Dog Backpacks, Carriers &amp; Pet Travel Products</t>
+        </is>
+      </c>
+      <c r="B3" s="8" t="inlineStr">
+        <is>
+          <t>Outward Hound</t>
+        </is>
+      </c>
+      <c r="C3" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" s="8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="inlineStr">
+        <is>
+          <t>Nina Ottosson By Outward Hound - Interactive Puzzle Game Dog Toys</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="inlineStr">
         <is>
           <t>Visit the Outward Hound Store</t>
         </is>
       </c>
-      <c r="C2" s="12" t="n">
-        <v>7</v>
-      </c>
-      <c r="D2" s="12" t="n">
+      <c r="C4" s="8" t="n">
+        <v>19</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="inlineStr">
+        <is>
+          <t>Outward Hound Fun Feeder Dog Bowl</t>
+        </is>
+      </c>
+      <c r="B5" s="8" t="inlineStr">
+        <is>
+          <t>Outward Hound</t>
+        </is>
+      </c>
+      <c r="C5" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="E2" s="12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="12" t="inlineStr">
-        <is>
-          <t>Outward Hound, Lightweight Dog Backpacks, Carriers &amp; Pet Travel Products</t>
-        </is>
-      </c>
-      <c r="B3" s="12" t="inlineStr">
-        <is>
-          <t>Outward Hound</t>
-        </is>
-      </c>
-      <c r="C3" s="12" t="n">
-        <v>6</v>
-      </c>
-      <c r="D3" s="12" t="n">
+      <c r="D5" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="E3" s="12" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="12" t="inlineStr">
-        <is>
-          <t>Nina Ottosson By Outward Hound - Interactive Puzzle Game Dog Toys</t>
-        </is>
-      </c>
-      <c r="B4" s="9" t="inlineStr">
+      <c r="E5" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="inlineStr">
+        <is>
+          <t>Outward Hound (4 pc. Multi-Pack) Invincibles Plush Stuffing-Less Dog Toys with Squeaker</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
         <is>
           <t>Visit the Outward Hound Store</t>
         </is>
       </c>
-      <c r="C4" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="12" t="n">
-        <v>4</v>
-      </c>
-      <c r="E4" s="12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="12" t="inlineStr">
-        <is>
-          <t>Outward Hound Fun Feeder Dog Bowl</t>
-        </is>
-      </c>
-      <c r="B5" s="12" t="inlineStr">
-        <is>
-          <t>Outward Hound</t>
-        </is>
-      </c>
-      <c r="C5" s="12" t="n">
-        <v>6</v>
-      </c>
-      <c r="D5" s="12" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" s="12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="12" t="inlineStr">
-        <is>
-          <t>Outward Hound (4 pc. Multi-Pack) Invincibles Plush Stuffing-Less Dog Toys with Squeaker</t>
-        </is>
-      </c>
-      <c r="B6" s="9" t="inlineStr">
-        <is>
-          <t>Visit the Outward Hound Store</t>
-        </is>
-      </c>
-      <c r="C6" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="12" t="n">
+      <c r="C6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -677,39 +647,45 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
     <col width="82.81640625" customWidth="1" style="3" min="1" max="1"/>
     <col width="25.7265625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="40.6328125" customWidth="1" style="3" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Product Title</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>Brand</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Style</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Size</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>Color</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>URL</t>
         </is>
       </c>
     </row>
@@ -844,7 +820,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1"/>
+  <autoFilter ref="A1:F6"/>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId21"/>
     <hyperlink ref="F3" r:id="rId22"/>

</xml_diff>

<commit_message>
Gets Selected Variation Style/Size/Color
Grabs the current selected variation style/size/color and logs it into the Logged sheet of Log workbook. The order of the pairs of variation types might be wrong, need to test more products to prove it. Seems pretty good, just need to add more products and URLs to test and find more bugs. Still kinda slow, lxml might make it a bit faster.
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="150" yWindow="2020" windowWidth="16670" windowHeight="7360" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Logged" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Actual" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Logged'!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Actual'!$A$1:$F$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Logged'!$B$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Actual'!$A$1:$I$6</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -101,14 +101,14 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
@@ -488,42 +488,60 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col width="82.7265625" customWidth="1" style="3" min="1" max="1"/>
-    <col width="25.6328125" customWidth="1" style="3" min="2" max="2"/>
+    <col width="82.7265625" customWidth="1" style="7" min="1" max="1"/>
+    <col width="25.6328125" customWidth="1" style="7" min="2" max="2"/>
+    <col width="11.7265625" customWidth="1" style="7" min="6" max="6"/>
+    <col width="12.453125" customWidth="1" style="7" min="7" max="7"/>
+    <col width="11.81640625" customWidth="1" style="7" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Product Title</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Brand</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
-        <is>
-          <t>Style</t>
-        </is>
-      </c>
-      <c r="D1" s="7" t="inlineStr">
-        <is>
-          <t>Size</t>
-        </is>
-      </c>
-      <c r="E1" s="7" t="inlineStr">
-        <is>
-          <t>Color</t>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Style Ct</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>Size Ct</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>Color Ct</t>
+        </is>
+      </c>
+      <c r="F1" s="5" t="inlineStr">
+        <is>
+          <t>Style Selected</t>
+        </is>
+      </c>
+      <c r="G1" s="5" t="inlineStr">
+        <is>
+          <t>Size Selected</t>
+        </is>
+      </c>
+      <c r="H1" s="5" t="inlineStr">
+        <is>
+          <t>Color Selected</t>
         </is>
       </c>
     </row>
@@ -533,9 +551,9 @@
           <t>Outward Hound Hide-A-Squirrel Squeaky Puzzle Plush Dog Toy - Hide and Seek Activity for Dogs</t>
         </is>
       </c>
-      <c r="B2" s="8" t="inlineStr">
-        <is>
-          <t>Outward Hound</t>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>Visit the Outward Hound Store</t>
         </is>
       </c>
       <c r="C2" s="8" t="n">
@@ -547,6 +565,17 @@
       <c r="E2" s="8" t="n">
         <v>0</v>
       </c>
+      <c r="F2" s="8" t="inlineStr">
+        <is>
+          <t>Squirrel</t>
+        </is>
+      </c>
+      <c r="G2" s="8" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="H2" s="8" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="8" t="inlineStr">
@@ -554,9 +583,9 @@
           <t>Outward Hound, Lightweight Dog Backpacks, Carriers &amp; Pet Travel Products</t>
         </is>
       </c>
-      <c r="B3" s="8" t="inlineStr">
-        <is>
-          <t>Outward Hound</t>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>Visit the Outward Hound Store</t>
         </is>
       </c>
       <c r="C3" s="8" t="n">
@@ -568,6 +597,21 @@
       <c r="E3" s="8" t="n">
         <v>3</v>
       </c>
+      <c r="F3" s="8" t="inlineStr">
+        <is>
+          <t>Treat Bag</t>
+        </is>
+      </c>
+      <c r="G3" s="8" t="inlineStr">
+        <is>
+          <t>One-Size</t>
+        </is>
+      </c>
+      <c r="H3" s="8" t="inlineStr">
+        <is>
+          <t>Grey</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="8" t="inlineStr">
@@ -575,7 +619,7 @@
           <t>Nina Ottosson By Outward Hound - Interactive Puzzle Game Dog Toys</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B4" s="4" t="inlineStr">
         <is>
           <t>Visit the Outward Hound Store</t>
         </is>
@@ -589,6 +633,17 @@
       <c r="E4" s="8" t="n">
         <v>0</v>
       </c>
+      <c r="F4" s="8" t="inlineStr">
+        <is>
+          <t>Dog Smart</t>
+        </is>
+      </c>
+      <c r="G4" s="8" t="inlineStr">
+        <is>
+          <t>Level 1 (Easy)</t>
+        </is>
+      </c>
+      <c r="H4" s="8" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="8" t="inlineStr">
@@ -596,9 +651,9 @@
           <t>Outward Hound Fun Feeder Dog Bowl</t>
         </is>
       </c>
-      <c r="B5" s="8" t="inlineStr">
-        <is>
-          <t>Outward Hound</t>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>Visit the Outward Hound Store</t>
         </is>
       </c>
       <c r="C5" s="8" t="n">
@@ -610,6 +665,17 @@
       <c r="E5" s="8" t="n">
         <v>0</v>
       </c>
+      <c r="F5" s="8" t="inlineStr">
+        <is>
+          <t>Purple Flower</t>
+        </is>
+      </c>
+      <c r="G5" s="8" t="inlineStr">
+        <is>
+          <t>Large/Regular</t>
+        </is>
+      </c>
+      <c r="H5" s="8" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="8" t="inlineStr">
@@ -617,7 +683,7 @@
           <t>Outward Hound (4 pc. Multi-Pack) Invincibles Plush Stuffing-Less Dog Toys with Squeaker</t>
         </is>
       </c>
-      <c r="B6" s="5" t="inlineStr">
+      <c r="B6" s="4" t="inlineStr">
         <is>
           <t>Visit the Outward Hound Store</t>
         </is>
@@ -631,9 +697,12 @@
       <c r="E6" s="8" t="n">
         <v>0</v>
       </c>
+      <c r="F6" s="8" t="n"/>
+      <c r="G6" s="8" t="n"/>
+      <c r="H6" s="8" t="n"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1"/>
+  <autoFilter ref="B1:H1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -644,46 +713,64 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col width="82.81640625" customWidth="1" style="3" min="1" max="1"/>
-    <col width="25.7265625" customWidth="1" style="3" min="2" max="2"/>
-    <col width="40.6328125" customWidth="1" style="3" min="6" max="6"/>
+    <col width="82.81640625" customWidth="1" style="7" min="1" max="1"/>
+    <col width="25.7265625" customWidth="1" style="7" min="2" max="2"/>
+    <col width="10.6328125" customWidth="1" style="7" min="6" max="6"/>
+    <col width="11.90625" customWidth="1" style="7" min="7" max="7"/>
+    <col width="10.90625" customWidth="1" style="7" min="8" max="8"/>
+    <col width="40.6328125" customWidth="1" style="7" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Product Title</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Brand</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
-        <is>
-          <t>Style</t>
-        </is>
-      </c>
-      <c r="D1" s="7" t="inlineStr">
-        <is>
-          <t>Size</t>
-        </is>
-      </c>
-      <c r="E1" s="7" t="inlineStr">
-        <is>
-          <t>Color</t>
-        </is>
-      </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Style Ct</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>Size Ct</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>Color Ct</t>
+        </is>
+      </c>
+      <c r="F1" s="5" t="inlineStr">
+        <is>
+          <t>Style Selected</t>
+        </is>
+      </c>
+      <c r="G1" s="5" t="inlineStr">
+        <is>
+          <t>Size Selected</t>
+        </is>
+      </c>
+      <c r="H1" s="5" t="inlineStr">
+        <is>
+          <t>Color Selected</t>
+        </is>
+      </c>
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
@@ -709,14 +796,24 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Squirrel</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
         <is>
           <t>https://www.amazon.com/dp/B005VS9WO6</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Outward Hound, Lightweight Dog Backpacks, Carriers &amp; Pet Travel Products</t>
         </is>
@@ -735,14 +832,29 @@
       <c r="E3" t="n">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="inlineStr">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Treat Bag</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>One-Size</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Grey</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
         <is>
           <t>https://www.amazon.com/dp/B0081XINMA</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>Nina Ottosson By Outward Hound - Interactive Puzzle Game Dog Toys</t>
         </is>
@@ -761,14 +873,24 @@
       <c r="E4" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="1" t="inlineStr">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Dog Smart</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Level 1 (Easy)</t>
+        </is>
+      </c>
+      <c r="I4" s="1" t="inlineStr">
         <is>
           <t>https://www.amazon.com/dp/B0711Y9Y8W</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>Outward Hound Fun Feeder Dog Bowl</t>
         </is>
@@ -787,14 +909,24 @@
       <c r="E5" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="1" t="inlineStr">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Purple Flower</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Large/Regular</t>
+        </is>
+      </c>
+      <c r="I5" s="1" t="inlineStr">
         <is>
           <t>https://www.amazon.com/dp/B00FPKNRG4</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>Outward Hound (4 pc. Multi-Pack) Invincibles Plush Stuffing-Less Dog Toys with Squeaker</t>
         </is>
@@ -813,40 +945,40 @@
       <c r="E6" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="1" t="inlineStr">
+      <c r="I6" s="1" t="inlineStr">
         <is>
           <t>https://www.amazon.com/dp/B075FY228K</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F6"/>
+  <autoFilter ref="A1:I6"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId21"/>
-    <hyperlink ref="F3" r:id="rId22"/>
-    <hyperlink ref="F4" r:id="rId23"/>
-    <hyperlink ref="F5" r:id="rId24"/>
-    <hyperlink ref="F6" r:id="rId25"/>
-    <hyperlink ref="F2" r:id="rId21"/>
-    <hyperlink ref="F3" r:id="rId22"/>
-    <hyperlink ref="F4" r:id="rId23"/>
-    <hyperlink ref="F5" r:id="rId24"/>
-    <hyperlink ref="F6" r:id="rId25"/>
-    <hyperlink ref="F2" r:id="rId21"/>
-    <hyperlink ref="F3" r:id="rId22"/>
-    <hyperlink ref="F4" r:id="rId23"/>
-    <hyperlink ref="F5" r:id="rId24"/>
-    <hyperlink ref="F6" r:id="rId25"/>
-    <hyperlink ref="F2" r:id="rId21"/>
-    <hyperlink ref="F3" r:id="rId22"/>
-    <hyperlink ref="F4" r:id="rId23"/>
-    <hyperlink ref="F5" r:id="rId24"/>
-    <hyperlink ref="F6" r:id="rId25"/>
-    <hyperlink ref="F2" r:id="rId21"/>
-    <hyperlink ref="F3" r:id="rId22"/>
-    <hyperlink ref="F4" r:id="rId23"/>
-    <hyperlink ref="F5" r:id="rId24"/>
-    <hyperlink ref="F6" r:id="rId25"/>
+    <hyperlink ref="I2" r:id="rId21"/>
+    <hyperlink ref="I3" r:id="rId22"/>
+    <hyperlink ref="I4" r:id="rId23"/>
+    <hyperlink ref="I5" r:id="rId24"/>
+    <hyperlink ref="I6" r:id="rId25"/>
+    <hyperlink ref="I2" r:id="rId21"/>
+    <hyperlink ref="I3" r:id="rId22"/>
+    <hyperlink ref="I4" r:id="rId23"/>
+    <hyperlink ref="I5" r:id="rId24"/>
+    <hyperlink ref="I6" r:id="rId25"/>
+    <hyperlink ref="I2" r:id="rId21"/>
+    <hyperlink ref="I3" r:id="rId22"/>
+    <hyperlink ref="I4" r:id="rId23"/>
+    <hyperlink ref="I5" r:id="rId24"/>
+    <hyperlink ref="I6" r:id="rId25"/>
+    <hyperlink ref="I2" r:id="rId21"/>
+    <hyperlink ref="I3" r:id="rId22"/>
+    <hyperlink ref="I4" r:id="rId23"/>
+    <hyperlink ref="I5" r:id="rId24"/>
+    <hyperlink ref="I6" r:id="rId25"/>
+    <hyperlink ref="I2" r:id="rId21"/>
+    <hyperlink ref="I3" r:id="rId22"/>
+    <hyperlink ref="I4" r:id="rId23"/>
+    <hyperlink ref="I5" r:id="rId24"/>
+    <hyperlink ref="I6" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>